<commit_message>
interim changes to diagnose ccd errors
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/hrs_ccd_case_definition_v1.0_AAT.xlsx
+++ b/src/functionalTest/resources/hrs_ccd_case_definition_v1.0_AAT.xlsx
@@ -1059,16 +1059,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d\ mmm\ yyyy"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="168" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="169" formatCode="0"/>
-    <numFmt numFmtId="170" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1345,11 +1344,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF808080"/>
       <name val="Menlo"/>
       <family val="2"/>
@@ -1503,7 +1497,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="167">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1892,11 +1886,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1912,11 +1906,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1936,7 +1930,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1952,7 +1946,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2076,10 +2070,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2096,10 +2086,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="3" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2164,7 +2150,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2172,7 +2158,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2868,8 +2854,8 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4316,7 +4302,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4648,7 +4634,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J55" activeCellId="0" sqref="J55"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4736,9 +4722,9 @@
       <c r="N4" s="54"/>
       <c r="O4" s="54"/>
     </row>
-    <row r="5" s="55" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="143" t="n">
-        <v>44562</v>
+    <row r="5" s="55" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="50" t="n">
+        <v>44197</v>
       </c>
       <c r="C5" s="43" t="s">
         <v>40</v>
@@ -4772,7 +4758,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4788,7 +4774,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="143" t="s">
         <v>285</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -4800,8 +4786,8 @@
       <c r="D1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
       <c r="H1" s="91"/>
       <c r="I1" s="91"/>
       <c r="J1" s="91"/>
@@ -4833,22 +4819,22 @@
       <c r="K2" s="130"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="145" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="145" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="147" t="s">
+      <c r="C3" s="146" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="147" t="s">
+      <c r="D3" s="146" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="147" t="s">
+      <c r="E3" s="146" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="146" t="s">
+      <c r="F3" s="145" t="s">
         <v>282</v>
       </c>
       <c r="G3" s="91"/>
@@ -4868,7 +4854,7 @@
       <c r="D4" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="148" t="s">
+      <c r="E4" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F4" s="52" t="s">
@@ -4895,7 +4881,7 @@
       <c r="D5" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F5" s="52" t="s">
@@ -4913,7 +4899,7 @@
       <c r="D6" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="148" t="s">
+      <c r="E6" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F6" s="52" t="s">
@@ -4931,7 +4917,7 @@
       <c r="D7" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="148" t="s">
+      <c r="E7" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F7" s="52" t="s">
@@ -4949,7 +4935,7 @@
       <c r="D8" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="148" t="s">
+      <c r="E8" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F8" s="52" t="s">
@@ -4967,7 +4953,7 @@
       <c r="D9" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="148" t="s">
+      <c r="E9" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F9" s="52" t="s">
@@ -4985,7 +4971,7 @@
       <c r="D10" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="148" t="s">
+      <c r="E10" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F10" s="52" t="s">
@@ -5003,7 +4989,7 @@
       <c r="D11" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="148" t="s">
+      <c r="E11" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F11" s="52" t="s">
@@ -5021,7 +5007,7 @@
       <c r="D12" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="148" t="s">
+      <c r="E12" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F12" s="52" t="s">
@@ -5039,7 +5025,7 @@
       <c r="D13" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="148" t="s">
+      <c r="E13" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F13" s="52" t="s">
@@ -5091,7 +5077,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5154,13 +5140,13 @@
       <c r="B3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="149" t="s">
+      <c r="C3" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="149" t="s">
+      <c r="D3" s="147" t="s">
         <v>189</v>
       </c>
-      <c r="E3" s="149" t="s">
+      <c r="E3" s="147" t="s">
         <v>228</v>
       </c>
       <c r="F3" s="21" t="s">
@@ -5178,7 +5164,7 @@
       <c r="D4" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="E4" s="148" t="s">
+      <c r="E4" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F4" s="52" t="s">
@@ -5196,7 +5182,7 @@
       <c r="D5" s="52" t="s">
         <v>162</v>
       </c>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F5" s="52" t="s">
@@ -5214,7 +5200,7 @@
       <c r="D6" s="53" t="s">
         <v>165</v>
       </c>
-      <c r="E6" s="148" t="s">
+      <c r="E6" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F6" s="52" t="s">
@@ -5232,7 +5218,7 @@
       <c r="D7" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="E7" s="148" t="s">
+      <c r="E7" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F7" s="52" t="s">
@@ -5250,7 +5236,7 @@
       <c r="D8" s="61" t="s">
         <v>172</v>
       </c>
-      <c r="E8" s="148" t="s">
+      <c r="E8" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F8" s="52" t="s">
@@ -5289,31 +5275,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="150" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="150" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="150" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="150" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="150" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="150" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="150" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="148" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="148" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="148" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="148" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="148" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="148" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="148" width="14.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="256" style="12" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="149" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="153" t="s">
+      <c r="C1" s="151" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="154" t="s">
+      <c r="D1" s="152" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
     </row>
     <row r="2" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
@@ -5325,7 +5311,7 @@
       <c r="C2" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="D2" s="156" t="s">
+      <c r="D2" s="154" t="s">
         <v>291</v>
       </c>
       <c r="E2" s="18" t="s">
@@ -5334,29 +5320,29 @@
       <c r="F2" s="35" t="s">
         <v>281</v>
       </c>
-      <c r="G2" s="157"/>
-      <c r="H2" s="157"/>
-      <c r="I2" s="157"/>
-      <c r="J2" s="157"/>
-      <c r="K2" s="157"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="155"/>
+      <c r="K2" s="155"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="158" t="s">
+      <c r="A3" s="156" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="158" t="s">
+      <c r="B3" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="149" t="s">
+      <c r="C3" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="149" t="s">
+      <c r="D3" s="147" t="s">
         <v>292</v>
       </c>
-      <c r="E3" s="149" t="s">
+      <c r="E3" s="147" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="158" t="s">
+      <c r="F3" s="156" t="s">
         <v>282</v>
       </c>
     </row>
@@ -5371,7 +5357,7 @@
       <c r="D4" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="148" t="s">
+      <c r="E4" s="53" t="s">
         <v>284</v>
       </c>
       <c r="F4" s="52" t="s">
@@ -5409,7 +5395,7 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -5498,7 +5484,7 @@
       <c r="E4" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="F4" s="148" t="s">
+      <c r="F4" s="53" t="s">
         <v>284</v>
       </c>
       <c r="G4" s="52" t="s">
@@ -5519,7 +5505,7 @@
       <c r="E5" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="F5" s="148" t="s">
+      <c r="F5" s="53" t="s">
         <v>284</v>
       </c>
       <c r="G5" s="52" t="s">
@@ -5540,7 +5526,7 @@
       <c r="E6" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="F6" s="148" t="s">
+      <c r="F6" s="53" t="s">
         <v>284</v>
       </c>
       <c r="G6" s="52" t="s">
@@ -5580,49 +5566,49 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="157" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="161"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="159"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="162" t="s">
+      <c r="A2" s="160" t="s">
         <v>297</v>
       </c>
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="160" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="162" t="s">
+      <c r="C2" s="160" t="s">
         <v>299</v>
       </c>
-      <c r="D2" s="162" t="s">
+      <c r="D2" s="160" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="163" t="s">
+      <c r="A3" s="161" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="163" t="s">
+      <c r="B3" s="161" t="s">
         <v>302</v>
       </c>
-      <c r="C3" s="163" t="s">
+      <c r="C3" s="161" t="s">
         <v>303</v>
       </c>
-      <c r="D3" s="163" t="s">
+      <c r="D3" s="161" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="4" s="68" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="164" t="s">
+      <c r="A4" s="162" t="s">
         <v>305</v>
       </c>
-      <c r="B4" s="165" t="s">
+      <c r="B4" s="163" t="s">
         <v>306</v>
       </c>
-      <c r="C4" s="165" t="s">
+      <c r="C4" s="163" t="s">
         <v>307</v>
       </c>
       <c r="D4" s="26" t="s">
@@ -5630,10 +5616,10 @@
       </c>
     </row>
     <row r="5" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="166"/>
-      <c r="B5" s="167"/>
-      <c r="C5" s="167"/>
-      <c r="D5" s="168"/>
+      <c r="A5" s="164"/>
+      <c r="B5" s="165"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="166"/>
     </row>
     <row r="6" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -9566,7 +9552,7 @@
   <dimension ref="A1:IU18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="D55" activeCellId="0" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10509,7 +10495,7 @@
   </sheetPr>
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -10929,7 +10915,7 @@
   </sheetPr>
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix up system user to have strict email format
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/hrs_ccd_case_definition_v1.0_AAT.xlsx
+++ b/src/functionalTest/resources/hrs_ccd_case_definition_v1.0_AAT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -1067,7 +1067,7 @@
     <numFmt numFmtId="168" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="169" formatCode="0"/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="42">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1335,11 +1335,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="10"/>
-      <color rgb="FF0563C1"/>
+      <color rgb="FF6A8759"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1353,6 +1352,14 @@
       <sz val="10"/>
       <color rgb="FF6A8759"/>
       <name val="Menlo"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1484,7 +1491,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2062,8 +2069,8 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2162,7 +2169,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="41" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2249,7 +2256,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4301,8 +4308,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4390,8 +4397,12 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="89"/>
+      <c r="A5" s="50"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="141"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="52"/>
     </row>
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
remove caseworker-hrs role and create role in idam script only
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/hrs_ccd_case_definition_v1.0_AAT.xlsx
+++ b/src/functionalTest/resources/hrs_ccd_case_definition_v1.0_AAT.xlsx
@@ -1067,7 +1067,7 @@
     <numFmt numFmtId="168" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="169" formatCode="0"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1336,13 +1336,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF6A8759"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF808080"/>
       <name val="Menlo"/>
       <family val="2"/>
@@ -1491,7 +1484,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1504,7 +1497,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="166">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2069,10 +2062,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2157,7 +2146,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2165,11 +2154,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="41" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2257,7 +2246,7 @@
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="5:5 D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2377,7 +2366,7 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="1" sqref="5:5 J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2519,7 +2508,7 @@
   <dimension ref="A1:N1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="1" sqref="5:5 H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2862,7 +2851,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="1" sqref="5:5 A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3065,7 +3054,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3353,7 +3342,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3630,7 +3619,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+      <selection pane="topLeft" activeCell="A50" activeCellId="1" sqref="5:5 A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3733,7 +3722,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4008,7 +3997,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4309,7 +4298,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="5:5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4396,10 +4385,10 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="50"/>
       <c r="B5" s="61"/>
-      <c r="C5" s="141"/>
+      <c r="C5" s="140"/>
       <c r="D5" s="140"/>
       <c r="E5" s="43"/>
       <c r="F5" s="52"/>
@@ -4428,7 +4417,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="5:5 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4484,7 +4473,7 @@
       <c r="C3" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="142" t="s">
+      <c r="D3" s="141" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="92" t="s">
@@ -4521,7 +4510,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="1" sqref="5:5 F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4645,7 +4634,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="5:5 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4769,7 +4758,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="5:5 C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4785,7 +4774,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="142" t="s">
         <v>285</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -4797,8 +4786,8 @@
       <c r="D1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
       <c r="H1" s="91"/>
       <c r="I1" s="91"/>
       <c r="J1" s="91"/>
@@ -4830,22 +4819,22 @@
       <c r="K2" s="130"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="145" t="s">
+      <c r="B3" s="144" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="145" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="146" t="s">
+      <c r="D3" s="145" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="146" t="s">
+      <c r="E3" s="145" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="145" t="s">
+      <c r="F3" s="144" t="s">
         <v>282</v>
       </c>
       <c r="G3" s="91"/>
@@ -5088,7 +5077,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="5:5 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5151,13 +5140,13 @@
       <c r="B3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="147" t="s">
+      <c r="C3" s="146" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="147" t="s">
+      <c r="D3" s="146" t="s">
         <v>189</v>
       </c>
-      <c r="E3" s="147" t="s">
+      <c r="E3" s="146" t="s">
         <v>228</v>
       </c>
       <c r="F3" s="21" t="s">
@@ -5281,36 +5270,36 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="5:5 E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="148" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="148" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="148" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="148" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="148" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="148" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="148" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="147" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="147" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="147" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="147" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="147" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="147" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="147" width="14.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="256" style="12" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="148" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="150" t="s">
+      <c r="B1" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="151" t="s">
+      <c r="C1" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="152" t="s">
+      <c r="D1" s="151" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
     </row>
     <row r="2" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
@@ -5322,7 +5311,7 @@
       <c r="C2" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="D2" s="154" t="s">
+      <c r="D2" s="153" t="s">
         <v>291</v>
       </c>
       <c r="E2" s="18" t="s">
@@ -5331,29 +5320,29 @@
       <c r="F2" s="35" t="s">
         <v>281</v>
       </c>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="155"/>
-      <c r="J2" s="155"/>
-      <c r="K2" s="155"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="156" t="s">
+      <c r="B3" s="155" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="147" t="s">
+      <c r="C3" s="146" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="147" t="s">
+      <c r="D3" s="146" t="s">
         <v>292</v>
       </c>
-      <c r="E3" s="147" t="s">
+      <c r="E3" s="146" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="156" t="s">
+      <c r="F3" s="155" t="s">
         <v>282</v>
       </c>
     </row>
@@ -5407,7 +5396,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="1" sqref="5:5 F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5564,7 +5553,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="1" sqref="5:5 E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5577,49 +5566,49 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="156" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="159"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="158"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="159" t="s">
         <v>297</v>
       </c>
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="159" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="160" t="s">
+      <c r="C2" s="159" t="s">
         <v>299</v>
       </c>
-      <c r="D2" s="160" t="s">
+      <c r="D2" s="159" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="160" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="160" t="s">
         <v>302</v>
       </c>
-      <c r="C3" s="161" t="s">
+      <c r="C3" s="160" t="s">
         <v>303</v>
       </c>
-      <c r="D3" s="161" t="s">
+      <c r="D3" s="160" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="4" s="68" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="162" t="s">
+      <c r="A4" s="161" t="s">
         <v>305</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="162" t="s">
         <v>306</v>
       </c>
-      <c r="C4" s="163" t="s">
+      <c r="C4" s="162" t="s">
         <v>307</v>
       </c>
       <c r="D4" s="26" t="s">
@@ -5627,10 +5616,10 @@
       </c>
     </row>
     <row r="5" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="164"/>
-      <c r="B5" s="165"/>
-      <c r="C5" s="165"/>
-      <c r="D5" s="166"/>
+      <c r="A5" s="163"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="165"/>
     </row>
     <row r="6" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5655,7 +5644,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5813,7 +5802,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="5:5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5989,7 +5978,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="5:5 D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9563,7 +9552,7 @@
   <dimension ref="A1:IU18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D55" activeCellId="0" sqref="D55"/>
+      <selection pane="topLeft" activeCell="D55" activeCellId="1" sqref="5:5 D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10374,7 +10363,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="5:5 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10507,7 +10496,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10927,7 +10916,7 @@
   <dimension ref="A1:AG34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+      <selection pane="topLeft" activeCell="K12" activeCellId="1" sqref="5:5 K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
remove user profile from ccd definition
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/hrs_ccd_case_definition_v1.0_AAT.xlsx
+++ b/src/functionalTest/resources/hrs_ccd_case_definition_v1.0_AAT.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="308">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -939,9 +939,6 @@
   </si>
   <si>
     <t xml:space="preserve">WorkBasketDefaultState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hrs.tester@hmcts.net</t>
   </si>
   <si>
     <t xml:space="preserve">CaseRoles</t>
@@ -2246,7 +2243,7 @@
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="5:5 D7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="4:4 D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2366,7 +2363,7 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="1" sqref="5:5 J3"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="1" sqref="4:4 J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2508,7 +2505,7 @@
   <dimension ref="A1:N1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="1" sqref="5:5 H9"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="1" sqref="4:4 H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2851,7 +2848,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="1" sqref="5:5 A33"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="1" sqref="4:4 A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3054,7 +3051,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3342,7 +3339,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3619,7 +3616,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="1" sqref="5:5 A50"/>
+      <selection pane="topLeft" activeCell="A50" activeCellId="1" sqref="4:4 A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3722,7 +3719,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3997,7 +3994,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4298,7 +4295,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="5:5"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4368,22 +4365,12 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="50" t="n">
-        <v>44197</v>
-      </c>
+      <c r="A4" s="50"/>
       <c r="B4" s="61"/>
-      <c r="C4" s="140" t="s">
-        <v>274</v>
-      </c>
-      <c r="D4" s="140" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="52" t="s">
-        <v>54</v>
-      </c>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="50"/>
@@ -4396,9 +4383,6 @@
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="hrs.tester@hmcts.net"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4417,7 +4401,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="5:5 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="4:4 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4429,7 +4413,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>10</v>
@@ -4451,16 +4435,16 @@
         <v>14</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>276</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4510,7 +4494,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="1" sqref="5:5 F26"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="1" sqref="4:4 F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4634,7 +4618,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="5:5 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4650,7 +4634,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>10</v>
@@ -4671,13 +4655,13 @@
         <v>14</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="35" t="s">
         <v>280</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4694,7 +4678,7 @@
         <v>228</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" s="55" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4706,10 +4690,10 @@
         <v>40</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F4" s="54"/>
       <c r="G4" s="54"/>
@@ -4730,10 +4714,10 @@
         <v>40</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" s="55" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4758,7 +4742,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="5:5 C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="4:4 C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4775,7 +4759,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="142" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>10</v>
@@ -4801,16 +4785,16 @@
         <v>14</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>287</v>
-      </c>
       <c r="E2" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="35" t="s">
         <v>280</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>281</v>
       </c>
       <c r="G2" s="130"/>
       <c r="H2" s="130"/>
@@ -4835,7 +4819,7 @@
         <v>228</v>
       </c>
       <c r="F3" s="144" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G3" s="91"/>
       <c r="H3" s="91"/>
@@ -4855,10 +4839,10 @@
         <v>76</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
@@ -4882,10 +4866,10 @@
         <v>80</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4900,10 +4884,10 @@
         <v>84</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4918,10 +4902,10 @@
         <v>86</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4936,10 +4920,10 @@
         <v>89</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4954,10 +4938,10 @@
         <v>91</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4972,10 +4956,10 @@
         <v>93</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4990,10 +4974,10 @@
         <v>95</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5008,10 +4992,10 @@
         <v>97</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5026,10 +5010,10 @@
         <v>101</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5077,7 +5061,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="5:5 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5094,7 +5078,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>10</v>
@@ -5116,16 +5100,16 @@
         <v>14</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="35" t="s">
         <v>280</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>281</v>
       </c>
       <c r="G2" s="48"/>
       <c r="H2" s="48"/>
@@ -5150,7 +5134,7 @@
         <v>228</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5165,10 +5149,10 @@
         <v>158</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5183,10 +5167,10 @@
         <v>162</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5201,10 +5185,10 @@
         <v>165</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5219,10 +5203,10 @@
         <v>168</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5237,10 +5221,10 @@
         <v>172</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5270,7 +5254,7 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="5:5 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5287,7 +5271,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="148" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B1" s="149" t="s">
         <v>10</v>
@@ -5309,16 +5293,16 @@
         <v>14</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D2" s="153" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="35" t="s">
         <v>280</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>281</v>
       </c>
       <c r="G2" s="154"/>
       <c r="H2" s="154"/>
@@ -5337,13 +5321,13 @@
         <v>51</v>
       </c>
       <c r="D3" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E3" s="146" t="s">
         <v>228</v>
       </c>
       <c r="F3" s="155" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" s="55" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5358,10 +5342,10 @@
         <v>54</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
@@ -5396,7 +5380,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="1" sqref="5:5 F4"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5413,7 +5397,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>10</v>
@@ -5432,19 +5416,19 @@
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>105</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5467,7 +5451,7 @@
         <v>228</v>
       </c>
       <c r="G3" s="77" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" s="55" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5485,10 +5469,10 @@
         <v>118</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" s="55" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5506,10 +5490,10 @@
         <v>115</v>
       </c>
       <c r="F5" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" s="55" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5527,10 +5511,10 @@
         <v>121</v>
       </c>
       <c r="F6" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -5553,7 +5537,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="1" sqref="5:5 E34"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="1" sqref="4:4 E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5567,7 +5551,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="156" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B1" s="157"/>
       <c r="C1" s="157"/>
@@ -5575,44 +5559,44 @@
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="159" t="s">
+        <v>296</v>
+      </c>
+      <c r="B2" s="159" t="s">
         <v>297</v>
       </c>
-      <c r="B2" s="159" t="s">
+      <c r="C2" s="159" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="159" t="s">
+      <c r="D2" s="159" t="s">
         <v>299</v>
-      </c>
-      <c r="D2" s="159" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="160" t="s">
+        <v>300</v>
+      </c>
+      <c r="B3" s="160" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="160" t="s">
+      <c r="C3" s="160" t="s">
         <v>302</v>
       </c>
-      <c r="C3" s="160" t="s">
+      <c r="D3" s="160" t="s">
         <v>303</v>
-      </c>
-      <c r="D3" s="160" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="4" s="68" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="161" t="s">
+        <v>304</v>
+      </c>
+      <c r="B4" s="162" t="s">
         <v>305</v>
       </c>
-      <c r="B4" s="162" t="s">
+      <c r="C4" s="162" t="s">
         <v>306</v>
       </c>
-      <c r="C4" s="162" t="s">
+      <c r="D4" s="26" t="s">
         <v>307</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="5" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5644,7 +5628,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5802,7 +5786,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="5:5"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="1" sqref="4:4 D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5978,7 +5962,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="5:5 D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="4:4 D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9552,7 +9536,7 @@
   <dimension ref="A1:IU18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D55" activeCellId="1" sqref="5:5 D55"/>
+      <selection pane="topLeft" activeCell="D55" activeCellId="1" sqref="4:4 D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10363,7 +10347,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="5:5 D9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="4:4 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10496,7 +10480,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10916,7 +10900,7 @@
   <dimension ref="A1:AG34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="1" sqref="5:5 K12"/>
+      <selection pane="topLeft" activeCell="K12" activeCellId="1" sqref="4:4 K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Revert "remove user profile from ccd definition"
This reverts commit cd6a22d2a22733934e69814fd432bc7a989b5af0.
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/hrs_ccd_case_definition_v1.0_AAT.xlsx
+++ b/src/functionalTest/resources/hrs_ccd_case_definition_v1.0_AAT.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="309">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -939,6 +939,9 @@
   </si>
   <si>
     <t xml:space="preserve">WorkBasketDefaultState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hrs.tester@hmcts.net</t>
   </si>
   <si>
     <t xml:space="preserve">CaseRoles</t>
@@ -2243,7 +2246,7 @@
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="4:4 D7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="5:5 D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2363,7 +2366,7 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="1" sqref="4:4 J3"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="1" sqref="5:5 J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2505,7 +2508,7 @@
   <dimension ref="A1:N1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="1" sqref="4:4 H9"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="1" sqref="5:5 H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2848,7 +2851,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="1" sqref="4:4 A33"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="1" sqref="5:5 A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3051,7 +3054,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3339,7 +3342,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3616,7 +3619,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="1" sqref="4:4 A50"/>
+      <selection pane="topLeft" activeCell="A50" activeCellId="1" sqref="5:5 A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3719,7 +3722,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3994,7 +3997,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4295,7 +4298,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="5:5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4365,12 +4368,22 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="50"/>
+      <c r="A4" s="50" t="n">
+        <v>44197</v>
+      </c>
       <c r="B4" s="61"/>
-      <c r="C4" s="140"/>
-      <c r="D4" s="140"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="52"/>
+      <c r="C4" s="140" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="140" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="50"/>
@@ -4383,6 +4396,9 @@
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" display="hrs.tester@hmcts.net"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4401,7 +4417,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="4:4 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="5:5 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4413,7 +4429,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>10</v>
@@ -4435,16 +4451,16 @@
         <v>14</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4494,7 +4510,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="1" sqref="4:4 F26"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="1" sqref="5:5 F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4618,7 +4634,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="5:5 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4634,7 +4650,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>10</v>
@@ -4655,13 +4671,13 @@
         <v>14</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4678,7 +4694,7 @@
         <v>228</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" s="55" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4690,10 +4706,10 @@
         <v>40</v>
       </c>
       <c r="D4" s="53" t="s">
+        <v>283</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>282</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>281</v>
       </c>
       <c r="F4" s="54"/>
       <c r="G4" s="54"/>
@@ -4714,10 +4730,10 @@
         <v>40</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" s="55" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4742,7 +4758,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="4:4 C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="5:5 C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4759,7 +4775,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="142" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>10</v>
@@ -4785,16 +4801,16 @@
         <v>14</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G2" s="130"/>
       <c r="H2" s="130"/>
@@ -4819,7 +4835,7 @@
         <v>228</v>
       </c>
       <c r="F3" s="144" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G3" s="91"/>
       <c r="H3" s="91"/>
@@ -4839,10 +4855,10 @@
         <v>76</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
@@ -4866,10 +4882,10 @@
         <v>80</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4884,10 +4900,10 @@
         <v>84</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4902,10 +4918,10 @@
         <v>86</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4920,10 +4936,10 @@
         <v>89</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4938,10 +4954,10 @@
         <v>91</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4956,10 +4972,10 @@
         <v>93</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4974,10 +4990,10 @@
         <v>95</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4992,10 +5008,10 @@
         <v>97</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5010,10 +5026,10 @@
         <v>101</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5061,7 +5077,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="5:5 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5078,7 +5094,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>10</v>
@@ -5100,16 +5116,16 @@
         <v>14</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G2" s="48"/>
       <c r="H2" s="48"/>
@@ -5134,7 +5150,7 @@
         <v>228</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5149,10 +5165,10 @@
         <v>158</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5167,10 +5183,10 @@
         <v>162</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5185,10 +5201,10 @@
         <v>165</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5203,10 +5219,10 @@
         <v>168</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5221,10 +5237,10 @@
         <v>172</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5254,7 +5270,7 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="5:5 E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5271,7 +5287,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="148" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B1" s="149" t="s">
         <v>10</v>
@@ -5293,16 +5309,16 @@
         <v>14</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D2" s="153" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G2" s="154"/>
       <c r="H2" s="154"/>
@@ -5321,13 +5337,13 @@
         <v>51</v>
       </c>
       <c r="D3" s="146" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E3" s="146" t="s">
         <v>228</v>
       </c>
       <c r="F3" s="155" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" s="55" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5342,10 +5358,10 @@
         <v>54</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
@@ -5380,7 +5396,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="1" sqref="5:5 F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5397,7 +5413,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>10</v>
@@ -5416,19 +5432,19 @@
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="18" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>105</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5451,7 +5467,7 @@
         <v>228</v>
       </c>
       <c r="G3" s="77" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" s="55" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5469,10 +5485,10 @@
         <v>118</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" s="55" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5490,10 +5506,10 @@
         <v>115</v>
       </c>
       <c r="F5" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" s="55" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5511,10 +5527,10 @@
         <v>121</v>
       </c>
       <c r="F6" s="53" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -5537,7 +5553,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="1" sqref="4:4 E34"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="1" sqref="5:5 E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5551,7 +5567,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="156" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B1" s="157"/>
       <c r="C1" s="157"/>
@@ -5559,44 +5575,44 @@
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="159" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B2" s="159" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C2" s="159" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D2" s="159" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="160" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B3" s="160" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C3" s="160" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D3" s="160" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" s="68" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="161" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B4" s="162" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C4" s="162" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5628,7 +5644,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5786,7 +5802,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="1" sqref="4:4 D5"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="5:5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5962,7 +5978,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="4:4 D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="5:5 D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9536,7 +9552,7 @@
   <dimension ref="A1:IU18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D55" activeCellId="1" sqref="4:4 D55"/>
+      <selection pane="topLeft" activeCell="D55" activeCellId="1" sqref="5:5 D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10347,7 +10363,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="4:4 D9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="5:5 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10480,7 +10496,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="5:5 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10900,7 +10916,7 @@
   <dimension ref="A1:AG34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="1" sqref="4:4 K12"/>
+      <selection pane="topLeft" activeCell="K12" activeCellId="1" sqref="5:5 K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>